<commit_message>
Update final entrants in each challenge
Update final entrants in each challenge
</commit_message>
<xml_diff>
--- a/30-DaysOfCode.xlsx
+++ b/30-DaysOfCode.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Day</t>
   </si>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>complete</t>
-  </si>
-  <si>
-    <t>@9:17am</t>
   </si>
 </sst>
 </file>
@@ -342,94 +339,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>26184</c:v>
+                  <c:v>26250</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15199</c:v>
+                  <c:v>15248</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15788</c:v>
+                  <c:v>15842</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14814</c:v>
+                  <c:v>14872</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10811</c:v>
+                  <c:v>10861</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10739</c:v>
+                  <c:v>10795</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10681</c:v>
+                  <c:v>10742</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10786</c:v>
+                  <c:v>10860</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8109</c:v>
+                  <c:v>8176</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8665</c:v>
+                  <c:v>8732</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7969</c:v>
+                  <c:v>8042</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6281</c:v>
+                  <c:v>6348</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6091</c:v>
+                  <c:v>6161</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5560</c:v>
+                  <c:v>5632</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5297</c:v>
+                  <c:v>5371</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5101</c:v>
+                  <c:v>5192</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4508</c:v>
+                  <c:v>4614</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4278</c:v>
+                  <c:v>4373</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3972</c:v>
+                  <c:v>4088</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4021</c:v>
+                  <c:v>4125</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3869</c:v>
+                  <c:v>4002</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3662</c:v>
+                  <c:v>3806</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3519</c:v>
+                  <c:v>3694</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3095</c:v>
+                  <c:v>3300</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3017</c:v>
+                  <c:v>3230</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3624</c:v>
+                  <c:v>3850</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2905</c:v>
+                  <c:v>3187</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2402</c:v>
+                  <c:v>2768</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1876</c:v>
+                  <c:v>2307</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>958</c:v>
+                  <c:v>2109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1493,7 +1490,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1514,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>26184</v>
+        <v>26250</v>
       </c>
       <c r="C2" s="1">
         <f>B2/$B$2</f>
@@ -1526,11 +1523,11 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>15199</v>
+        <v>15248</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C31" si="0">B3/$B$2</f>
-        <v>0.58046898869538655</v>
+        <v>0.58087619047619043</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1538,11 +1535,11 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>15788</v>
+        <v>15842</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
-        <v>0.60296364191872898</v>
+        <v>0.60350476190476188</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1550,11 +1547,11 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>14814</v>
+        <v>14872</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
-        <v>0.56576535288725938</v>
+        <v>0.56655238095238092</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1562,11 +1559,11 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>10811</v>
+        <v>10861</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
-        <v>0.41288573174457682</v>
+        <v>0.41375238095238093</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1574,11 +1571,11 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>10739</v>
+        <v>10795</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
-        <v>0.41013596089214788</v>
+        <v>0.41123809523809524</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1586,11 +1583,11 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>10681</v>
+        <v>10742</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
-        <v>0.40792086770546898</v>
+        <v>0.40921904761904759</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1598,11 +1595,11 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>10786</v>
+        <v>10860</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
-        <v>0.41193095019859455</v>
+        <v>0.4137142857142857</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1610,11 +1607,11 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8109</v>
+        <v>8176</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
-        <v>0.30969294225481209</v>
+        <v>0.31146666666666667</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1622,11 +1619,11 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>8665</v>
+        <v>8732</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
-        <v>0.33092728383745801</v>
+        <v>0.33264761904761903</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1634,11 +1631,11 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>7969</v>
+        <v>8042</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
-        <v>0.30434616559731131</v>
+        <v>0.30636190476190478</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1646,11 +1643,11 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>6281</v>
+        <v>6348</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
-        <v>0.23987931561258785</v>
+        <v>0.24182857142857142</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1658,11 +1655,11 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>6091</v>
+        <v>6161</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
-        <v>0.23262297586312253</v>
+        <v>0.23470476190476192</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1670,11 +1667,11 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>5560</v>
+        <v>5632</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
-        <v>0.21234341582645891</v>
+        <v>0.21455238095238094</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1682,11 +1679,11 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>5297</v>
+        <v>5371</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
-        <v>0.20229911396272532</v>
+        <v>0.2046095238095238</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1694,11 +1691,11 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>5101</v>
+        <v>5192</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
-        <v>0.19481362664222426</v>
+        <v>0.19779047619047618</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1706,11 +1703,11 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>4508</v>
+        <v>4614</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
-        <v>0.1721662083715246</v>
+        <v>0.17577142857142858</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1718,11 +1715,11 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>4278</v>
+        <v>4373</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
-        <v>0.16338221814848763</v>
+        <v>0.16659047619047618</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1730,11 +1727,11 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>3972</v>
+        <v>4088</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
-        <v>0.15169569202566452</v>
+        <v>0.15573333333333333</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1742,11 +1739,11 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>4021</v>
+        <v>4125</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
-        <v>0.1535670638557898</v>
+        <v>0.15714285714285714</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1754,11 +1751,11 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>3869</v>
+        <v>4002</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="0"/>
-        <v>0.14776199205621754</v>
+        <v>0.15245714285714285</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1766,11 +1763,11 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>3662</v>
+        <v>3806</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
-        <v>0.13985640085548426</v>
+        <v>0.1449904761904762</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1778,11 +1775,11 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>3519</v>
+        <v>3694</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
-        <v>0.13439505041246563</v>
+        <v>0.14072380952380953</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1790,11 +1787,11 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>3095</v>
+        <v>3300</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
-        <v>0.11820195539260617</v>
+        <v>0.12571428571428572</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1802,11 +1799,11 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>3017</v>
+        <v>3230</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="0"/>
-        <v>0.11522303696914146</v>
+        <v>0.12304761904761904</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1814,11 +1811,11 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>3624</v>
+        <v>3850</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="0"/>
-        <v>0.1384051329055912</v>
+        <v>0.14666666666666667</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1826,11 +1823,11 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>2905</v>
+        <v>3187</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="0"/>
-        <v>0.11094561564314084</v>
+        <v>0.12140952380952381</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1838,11 +1835,11 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>2402</v>
+        <v>2768</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="0"/>
-        <v>9.1735410937977394E-2</v>
+        <v>0.10544761904761905</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1850,11 +1847,11 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>1876</v>
+        <v>2307</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="0"/>
-        <v>7.1646807210510241E-2</v>
+        <v>8.7885714285714289E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1862,11 +1859,11 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>958</v>
+        <v>2109</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="0"/>
-        <v>3.6587228842040943E-2</v>
+        <v>8.0342857142857146E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1878,7 +1875,7 @@
       </c>
       <c r="C32" s="1">
         <f>B32/$B$2</f>
-        <v>2.7650473571646808E-2</v>
+        <v>2.758095238095238E-2</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1886,15 +1883,13 @@
         <v>4</v>
       </c>
       <c r="B33">
-        <v>793</v>
+        <v>1734</v>
       </c>
       <c r="C33" s="1">
         <f>B33/$B$2</f>
-        <v>3.0285670638557898E-2</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>6.6057142857142856E-2</v>
+      </c>
+      <c r="D33" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>